<commit_message>
[!] dobne upravy product backlog-u
</commit_message>
<xml_diff>
--- a/Dokumentacie/Ostatne/New-Product_Backlog.xlsx
+++ b/Dokumentacie/Ostatne/New-Product_Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="141">
   <si>
     <t>#ID</t>
   </si>
@@ -120,71 +120,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Date:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                2012</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Last update:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   15.04.2012</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="26"/>
-        <color theme="0"/>
-        <rFont val="Square721 BT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">                          Product BackLog</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Note </t>
   </si>
   <si>
@@ -297,9 +232,6 @@
   </si>
   <si>
     <t>#35</t>
-  </si>
-  <si>
-    <t>LK</t>
   </si>
   <si>
     <t>working</t>
@@ -370,31 +302,6 @@
     <t xml:space="preserve">        C -        low   feature</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Estimate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - how time in unit Days</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">done </t>
   </si>
   <si>
@@ -601,6 +508,102 @@
   </si>
   <si>
     <t>Show Licence</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT - Lukáš Turský,    JK - Jozef Krajčovič  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Estimate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - how time , unit is  Days</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last update:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      15.04.2012</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Date:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">               2012</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="26"/>
+        <color theme="0"/>
+        <rFont val="Square721 BT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                            Product BackLog</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1019,13 +1022,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>419101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1419225</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>69696</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1045,6 +1048,652 @@
         <a:xfrm>
           <a:off x="790576" y="1562101"/>
           <a:ext cx="1647824" cy="650720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obrázok 3" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4235824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Obrázok 4" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4426324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Obrázok 5" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4616824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Obrázok 6" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4807324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Obrázok 7" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="5569324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Obrázok 8" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="5378824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Obrázok 9" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="5188324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Obrázok 10" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4997824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Obrázok 11" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="3854824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Obrázok 12" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="6331324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Obrázok 13" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="6521824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Obrázok 14" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="6712324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Obrázok 17" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="2711824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Obrázok 18" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="3473824"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Obrázok 19" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="3664324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Obrázok 20" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="4045324"/>
+          <a:ext cx="235324" cy="235324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Obrázok 21" descr="png-0094.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11609294" y="5759824"/>
+          <a:ext cx="235324" cy="235324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1341,10 +1990,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:L74"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1356,948 +2006,1037 @@
     <col min="10" max="10" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3"/>
+    <row r="1" spans="2:11">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" ht="6.75" customHeight="1"/>
+    <row r="3" spans="2:11" ht="33.75">
+      <c r="B3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:11">
+      <c r="B4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-    </row>
-    <row r="7" spans="2:11" ht="33.75">
-      <c r="B7" s="10" t="s">
+      <c r="F4" s="3"/>
+      <c r="I4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="I5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="I6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="45">
+        <v>432</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="45">
+        <v>5</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="46"/>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="I8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="48">
+        <v>420</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="48">
+        <v>3</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
+      <c r="B11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="48">
+        <v>410</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="48">
+        <v>5</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="49"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="48">
+        <v>389</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="48">
+        <v>4</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="49"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="48">
+        <v>365</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="48">
+        <v>3</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="38">
+        <v>320</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="38">
         <v>1</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="45">
-        <v>432</v>
-      </c>
-      <c r="G13" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="45">
-        <v>5</v>
-      </c>
-      <c r="I13" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="46"/>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="48">
-        <v>420</v>
-      </c>
-      <c r="G14" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="48">
-        <v>3</v>
-      </c>
-      <c r="I14" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="49"/>
+      <c r="I14" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="39"/>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>34</v>
       </c>
       <c r="D15" s="47"/>
       <c r="E15" s="48" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F15" s="48">
-        <v>410</v>
+        <v>480</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H15" s="48">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="48" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J15" s="49"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="48">
-        <v>389</v>
-      </c>
-      <c r="G16" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="48">
-        <v>4</v>
-      </c>
-      <c r="I16" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" s="49"/>
+      <c r="B16" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="38">
+        <v>300</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="38">
+        <v>1</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="39"/>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>36</v>
       </c>
       <c r="D17" s="47"/>
       <c r="E17" s="48" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F17" s="48">
-        <v>365</v>
+        <v>449</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H17" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J17" s="49"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>37</v>
       </c>
       <c r="D18" s="37"/>
       <c r="E18" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F18" s="38">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H18" s="38">
         <v>1</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J18" s="39"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="48">
-        <v>480</v>
-      </c>
-      <c r="G19" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="48">
+      <c r="B19" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="38">
+        <v>256</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="38">
         <v>1</v>
       </c>
-      <c r="I19" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="49"/>
+      <c r="I19" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="39"/>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="37" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="37"/>
+        <v>74</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>76</v>
+      </c>
       <c r="E20" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F20" s="38">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H20" s="38">
         <v>1</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="47" t="s">
+      <c r="B21" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="48">
-        <v>449</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="48">
+      <c r="D21" s="37"/>
+      <c r="E21" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="38">
+        <v>266</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="38">
         <v>1</v>
       </c>
-      <c r="I21" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J21" s="49"/>
+      <c r="I21" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="39"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="37" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F22" s="38">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H22" s="38">
         <v>1</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J22" s="39"/>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="37" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="37"/>
       <c r="E23" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F23" s="38">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H23" s="38">
         <v>1</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J23" s="39"/>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>81</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D24" s="37"/>
       <c r="E24" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F24" s="38">
-        <v>265</v>
+        <v>340</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H24" s="38">
         <v>1</v>
       </c>
       <c r="I24" s="38" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J24" s="39"/>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="37" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="38" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F25" s="38">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H25" s="38">
         <v>1</v>
       </c>
       <c r="I25" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="39"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="34">
+        <v>150</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="34">
+        <v>2</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="35"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="34">
+        <v>110</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="34">
+        <v>3</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="35"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="34">
+        <v>120</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="34">
+        <v>3</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" s="35"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="48">
+        <v>453</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="48">
+        <v>2</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29" s="49"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="48">
+        <v>489</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="48">
+        <v>2</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" s="49"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="47"/>
+      <c r="E31" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="48">
+        <v>451</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="48">
+        <v>1</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="49"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="38">
-        <v>267</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H26" s="38">
-        <v>1</v>
-      </c>
-      <c r="I26" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="38">
-        <v>300</v>
-      </c>
-      <c r="G27" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="38">
-        <v>1</v>
-      </c>
-      <c r="I27" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="38">
-        <v>340</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="38">
-        <v>1</v>
-      </c>
-      <c r="I28" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="38">
-        <v>261</v>
-      </c>
-      <c r="G29" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="38">
-        <v>1</v>
-      </c>
-      <c r="I29" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="34">
-        <v>150</v>
-      </c>
-      <c r="G30" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H30" s="34">
+      <c r="D32" s="47"/>
+      <c r="E32" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="48">
+        <v>452</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="48">
         <v>2</v>
       </c>
-      <c r="I30" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30" s="35"/>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="34">
-        <v>110</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="34">
-        <v>3</v>
-      </c>
-      <c r="I31" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="J31" s="35"/>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="34">
-        <v>120</v>
-      </c>
-      <c r="G32" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="34">
-        <v>3</v>
-      </c>
-      <c r="I32" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="J32" s="35"/>
+      <c r="I32" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="49"/>
     </row>
     <row r="33" spans="1:12">
       <c r="B33" s="47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="47"/>
+        <v>89</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>90</v>
+      </c>
       <c r="E33" s="48" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F33" s="48">
-        <v>453</v>
+        <v>436</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H33" s="48">
         <v>2</v>
       </c>
       <c r="I33" s="48" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="J33" s="49"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="B34" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="47" t="s">
+      <c r="B34" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="38">
+        <v>222</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="38">
+        <v>2</v>
+      </c>
+      <c r="I34" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="39"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="B35" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" s="48">
-        <v>489</v>
-      </c>
-      <c r="G34" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="48">
-        <v>2</v>
-      </c>
-      <c r="I34" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="J34" s="49"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="B35" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="48">
-        <v>451</v>
-      </c>
-      <c r="G35" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H35" s="48">
+      <c r="D35" s="33"/>
+      <c r="E35" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="34">
+        <v>159</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="34">
         <v>1</v>
       </c>
-      <c r="I35" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="J35" s="49"/>
+      <c r="I35" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="B36" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F36" s="48">
-        <v>452</v>
-      </c>
-      <c r="G36" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H36" s="48">
-        <v>2</v>
-      </c>
-      <c r="I36" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="J36" s="49"/>
+      <c r="B36" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="34">
+        <v>165</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="34">
+        <v>1</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36" s="35"/>
     </row>
     <row r="37" spans="1:12">
       <c r="B37" s="47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C37" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="47"/>
+      <c r="E37" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="48">
+        <v>478</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="48">
+        <v>1</v>
+      </c>
+      <c r="I37" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="J37" s="49"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="B38" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="47"/>
+      <c r="E38" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="48">
+        <v>452</v>
+      </c>
+      <c r="G38" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" s="48">
+        <v>1</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" s="49"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A39" s="26"/>
+      <c r="B39" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="42">
+        <v>234</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H39" s="42">
+        <v>1</v>
+      </c>
+      <c r="I39" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="43"/>
+      <c r="K39" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="L39" s="26"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="B40" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="B41" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="34">
+        <v>50</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="34">
+        <v>1</v>
+      </c>
+      <c r="I41" s="34"/>
+      <c r="J41" s="35"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="B42" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="34">
+        <v>60</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="34">
+        <v>4</v>
+      </c>
+      <c r="I42" s="34"/>
+      <c r="J42" s="35"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="B43" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="34">
+        <v>12</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="34">
+        <v>1</v>
+      </c>
+      <c r="I43" s="34"/>
+      <c r="J43" s="35"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="B44" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="48">
-        <v>436</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37" s="48">
-        <v>2</v>
-      </c>
-      <c r="I37" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="J37" s="49"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="B38" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="38">
-        <v>222</v>
-      </c>
-      <c r="G38" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="38">
-        <v>2</v>
-      </c>
-      <c r="I38" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="J38" s="39"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="B39" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="33"/>
-      <c r="E39" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F39" s="34">
-        <v>159</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H39" s="34">
-        <v>1</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="J39" s="35"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="B40" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F40" s="34">
-        <v>165</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H40" s="34">
-        <v>1</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="J40" s="35"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="B41" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="48">
-        <v>478</v>
-      </c>
-      <c r="G41" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H41" s="48">
-        <v>1</v>
-      </c>
-      <c r="I41" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="J41" s="49"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="B42" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="47"/>
-      <c r="E42" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="48">
-        <v>452</v>
-      </c>
-      <c r="G42" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H42" s="48">
-        <v>1</v>
-      </c>
-      <c r="I42" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" s="49"/>
-    </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A43" s="26"/>
-      <c r="B43" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="42">
-        <v>234</v>
-      </c>
-      <c r="G43" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H43" s="42">
-        <v>1</v>
-      </c>
-      <c r="I43" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="J43" s="43"/>
-      <c r="K43" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="L43" s="26"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="B44" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="17"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" s="34">
+        <v>44</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" s="34">
+        <v>5</v>
+      </c>
+      <c r="I44" s="34"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:12">
       <c r="B45" s="33" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D45" s="33"/>
       <c r="E45" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F45" s="34">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H45" s="34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:12">
       <c r="B46" s="33" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>92</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D46" s="33"/>
       <c r="E46" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F46" s="34">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H46" s="34">
         <v>4</v>
@@ -2307,116 +3046,116 @@
     </row>
     <row r="47" spans="1:12">
       <c r="B47" s="33" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F47" s="34">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H47" s="34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I47" s="34"/>
-      <c r="J47" s="35"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:12">
       <c r="B48" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>99</v>
       </c>
       <c r="D48" s="33"/>
       <c r="E48" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F48" s="34">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H48" s="34">
         <v>5</v>
       </c>
       <c r="I48" s="34"/>
-      <c r="J48" s="35"/>
+      <c r="J48" s="36"/>
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D49" s="33"/>
       <c r="E49" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F49" s="34">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H49" s="34">
         <v>5</v>
       </c>
       <c r="I49" s="34"/>
-      <c r="J49" s="35"/>
+      <c r="J49" s="36"/>
     </row>
     <row r="50" spans="2:10">
       <c r="B50" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D50" s="33"/>
       <c r="E50" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F50" s="34">
-        <v>77</v>
+        <v>198</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H50" s="34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I50" s="34"/>
-      <c r="J50" s="35"/>
+      <c r="J50" s="36"/>
     </row>
     <row r="51" spans="2:10">
       <c r="B51" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F51" s="34">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H51" s="34">
         <v>5</v>
@@ -2426,20 +3165,22 @@
     </row>
     <row r="52" spans="2:10">
       <c r="B52" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D52" s="33"/>
+        <v>106</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>107</v>
+      </c>
       <c r="E52" s="34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F52" s="34">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H52" s="34">
         <v>5</v>
@@ -2448,104 +3189,60 @@
       <c r="J52" s="36"/>
     </row>
     <row r="53" spans="2:10">
-      <c r="B53" s="33" t="s">
+      <c r="B53" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="22"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D53" s="33"/>
-      <c r="E53" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="34">
-        <v>11</v>
-      </c>
-      <c r="G53" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H53" s="34">
-        <v>5</v>
-      </c>
-      <c r="I53" s="34"/>
-      <c r="J53" s="36"/>
-    </row>
-    <row r="54" spans="2:10">
-      <c r="B54" s="33" t="s">
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="22"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C54" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="33"/>
-      <c r="E54" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F54" s="34">
-        <v>198</v>
-      </c>
-      <c r="G54" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H54" s="34">
-        <v>2</v>
-      </c>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-    </row>
-    <row r="55" spans="2:10">
-      <c r="B55" s="33" t="s">
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="22"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F55" s="34">
-        <v>125</v>
-      </c>
-      <c r="G55" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H55" s="34">
-        <v>5</v>
-      </c>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-    </row>
-    <row r="56" spans="2:10">
-      <c r="B56" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E56" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F56" s="34">
-        <v>159</v>
-      </c>
-      <c r="G56" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H56" s="34">
-        <v>5</v>
-      </c>
-      <c r="I56" s="34"/>
-      <c r="J56" s="36"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="22"/>
     </row>
     <row r="57" spans="2:10">
       <c r="B57" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
@@ -2558,7 +3255,7 @@
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -2571,7 +3268,7 @@
     </row>
     <row r="59" spans="2:10">
       <c r="B59" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
@@ -2584,7 +3281,7 @@
     </row>
     <row r="60" spans="2:10">
       <c r="B60" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -2597,7 +3294,7 @@
     </row>
     <row r="61" spans="2:10">
       <c r="B61" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -2609,9 +3306,7 @@
       <c r="J61" s="22"/>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="14" t="s">
-        <v>127</v>
-      </c>
+      <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="21"/>
@@ -2622,9 +3317,7 @@
       <c r="J62" s="22"/>
     </row>
     <row r="63" spans="2:10">
-      <c r="B63" s="14" t="s">
-        <v>128</v>
-      </c>
+      <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="21"/>
@@ -2635,9 +3328,7 @@
       <c r="J63" s="22"/>
     </row>
     <row r="64" spans="2:10">
-      <c r="B64" s="14" t="s">
-        <v>129</v>
-      </c>
+      <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="21"/>
@@ -2648,9 +3339,7 @@
       <c r="J64" s="22"/>
     </row>
     <row r="65" spans="2:10">
-      <c r="B65" s="14" t="s">
-        <v>130</v>
-      </c>
+      <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="21"/>
@@ -2705,61 +3394,26 @@
       <c r="J69" s="22"/>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="22"/>
-    </row>
-    <row r="71" spans="2:10">
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
-      <c r="H71" s="21"/>
-      <c r="I71" s="21"/>
-      <c r="J71" s="22"/>
-    </row>
-    <row r="72" spans="2:10">
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="21"/>
-      <c r="J72" s="22"/>
-    </row>
-    <row r="73" spans="2:10">
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="22"/>
-    </row>
-    <row r="74" spans="2:10">
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="24"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="24"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2769,19 +3423,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="B2:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:16" ht="27.75">
       <c r="B2" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -2817,13 +3471,17 @@
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2853,7 +3511,7 @@
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2889,7 +3547,7 @@
     </row>
     <row r="8" spans="2:16">
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2908,13 +3566,13 @@
     </row>
     <row r="9" spans="2:16">
       <c r="B9" s="31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
       <c r="F9" s="32" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
@@ -2929,13 +3587,13 @@
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
@@ -2950,13 +3608,13 @@
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -2988,7 +3646,7 @@
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>

</xml_diff>